<commit_message>
added electrical boilers FI Helsinki and renamed the CHP capacity file.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-chp.xlsx
+++ b/input/capacity/additional-units-chp.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="46">
   <si>
     <t xml:space="preserve">Node</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t xml:space="preserve">Electric boiler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hanasaari ja Salmisaari</t>
   </si>
   <si>
     <t xml:space="preserve">Tampere_dheat</t>
@@ -305,7 +308,7 @@
   <dimension ref="A1:J140"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B153" activeCellId="0" sqref="B153"/>
+      <selection pane="topLeft" activeCell="C150" activeCellId="0" sqref="C150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -489,18 +492,20 @@
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="n">
-        <v>100</v>
+        <v>240</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="J7" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
@@ -524,7 +529,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>15</v>
@@ -548,10 +553,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>13</v>
@@ -571,7 +576,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>12</v>
@@ -594,7 +599,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>18</v>
@@ -615,10 +620,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>13</v>
@@ -638,7 +643,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>14</v>
@@ -658,10 +663,10 @@
         <v>10</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>13</v>
@@ -681,10 +686,10 @@
         <v>10</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>13</v>
@@ -704,7 +709,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>14</v>
@@ -724,7 +729,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>17</v>
@@ -744,10 +749,10 @@
         <v>10</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>13</v>
@@ -767,10 +772,10 @@
         <v>10</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>13</v>
@@ -790,10 +795,10 @@
         <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>13</v>
@@ -813,7 +818,7 @@
         <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>12</v>
@@ -836,7 +841,7 @@
         <v>10</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>15</v>
@@ -856,7 +861,7 @@
         <v>10</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>14</v>
@@ -871,15 +876,15 @@
         <v>200</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>13</v>
@@ -894,12 +899,12 @@
         <v>220</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>14</v>
@@ -919,7 +924,7 @@
         <v>10</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>12</v>
@@ -942,7 +947,7 @@
         <v>10</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>15</v>
@@ -962,7 +967,7 @@
         <v>10</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>14</v>
@@ -982,10 +987,10 @@
         <v>10</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>13</v>
@@ -1005,10 +1010,10 @@
         <v>10</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>13</v>
@@ -1028,7 +1033,7 @@
         <v>10</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>12</v>
@@ -1051,7 +1056,7 @@
         <v>10</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>16</v>
@@ -1071,7 +1076,7 @@
         <v>10</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>14</v>
@@ -1088,13 +1093,13 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>13</v>
@@ -1111,13 +1116,13 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>13</v>
@@ -1134,10 +1139,10 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>16</v>
@@ -1154,10 +1159,10 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>14</v>
@@ -1174,10 +1179,10 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>17</v>
@@ -1194,13 +1199,13 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>13</v>
@@ -1217,13 +1222,13 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>13</v>
@@ -1240,13 +1245,13 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>13</v>
@@ -1263,10 +1268,10 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>16</v>
@@ -1283,10 +1288,10 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>14</v>
@@ -1303,13 +1308,13 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>13</v>
@@ -1326,13 +1331,13 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>13</v>
@@ -1349,10 +1354,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>16</v>
@@ -1369,10 +1374,10 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>14</v>
@@ -1389,10 +1394,10 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>12</v>
@@ -1412,13 +1417,13 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>13</v>
@@ -1435,13 +1440,13 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>13</v>
@@ -1458,10 +1463,10 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>15</v>
@@ -1478,10 +1483,10 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>12</v>
@@ -1501,13 +1506,13 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>13</v>
@@ -1524,10 +1529,10 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>15</v>
@@ -1544,10 +1549,10 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>14</v>
@@ -1564,10 +1569,10 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>12</v>
@@ -1587,13 +1592,13 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>13</v>
@@ -1610,13 +1615,13 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>13</v>
@@ -1633,13 +1638,13 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>13</v>
@@ -1656,10 +1661,10 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>15</v>
@@ -1676,10 +1681,10 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>14</v>
@@ -1696,10 +1701,10 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>16</v>
@@ -1716,16 +1721,16 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E64" s="3" t="n">
         <v>2040</v>
@@ -1737,16 +1742,16 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E65" s="3" t="n">
         <v>2040</v>
@@ -1760,16 +1765,16 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E66" s="3" t="n">
         <v>2040</v>
@@ -1783,16 +1788,16 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E67" s="3" t="n">
         <v>2040</v>
@@ -1804,16 +1809,16 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E68" s="3" t="n">
         <v>2040</v>
@@ -1825,16 +1830,16 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E69" s="3" t="n">
         <v>2040</v>
@@ -1846,16 +1851,16 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E70" s="3" t="n">
         <v>2040</v>
@@ -1869,16 +1874,16 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E71" s="3" t="n">
         <v>2040</v>
@@ -1892,16 +1897,16 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E72" s="3" t="n">
         <v>2040</v>
@@ -1913,16 +1918,16 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E73" s="3" t="n">
         <v>2040</v>
@@ -1934,16 +1939,16 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E74" s="3" t="n">
         <v>2040</v>
@@ -1954,16 +1959,16 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E75" s="3" t="n">
         <v>2040</v>
@@ -1977,16 +1982,16 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E76" s="3" t="n">
         <v>2040</v>
@@ -2000,16 +2005,16 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E77" s="3" t="n">
         <v>2040</v>
@@ -2020,16 +2025,16 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E78" s="3" t="n">
         <v>2040</v>
@@ -2040,16 +2045,16 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E79" s="3" t="n">
         <v>2040</v>
@@ -2060,16 +2065,16 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E80" s="3" t="n">
         <v>2040</v>
@@ -2083,16 +2088,16 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E81" s="3" t="n">
         <v>2040</v>
@@ -2106,16 +2111,16 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E82" s="3" t="n">
         <v>2040</v>
@@ -2129,16 +2134,16 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E83" s="3" t="n">
         <v>2040</v>
@@ -2149,16 +2154,16 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E84" s="3" t="n">
         <v>2040</v>
@@ -2169,16 +2174,16 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E85" s="3" t="n">
         <v>2040</v>
@@ -2189,16 +2194,16 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E86" s="3" t="n">
         <v>2040</v>
@@ -2212,16 +2217,16 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E87" s="3" t="n">
         <v>2040</v>
@@ -2235,16 +2240,16 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E88" s="3" t="n">
         <v>2040</v>
@@ -2258,16 +2263,16 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E89" s="3" t="n">
         <v>2040</v>
@@ -2278,16 +2283,16 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E90" s="3" t="n">
         <v>2040</v>
@@ -2298,16 +2303,16 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E91" s="3" t="n">
         <v>2040</v>
@@ -2318,16 +2323,16 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E92" s="3" t="n">
         <v>2040</v>
@@ -2338,16 +2343,16 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E93" s="3" t="n">
         <v>2040</v>
@@ -2361,16 +2366,16 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E94" s="3" t="n">
         <v>2040</v>
@@ -2384,16 +2389,16 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E95" s="3" t="n">
         <v>2040</v>
@@ -2404,16 +2409,16 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E96" s="3" t="n">
         <v>2040</v>
@@ -2424,16 +2429,16 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E97" s="3" t="n">
         <v>2040</v>
@@ -2442,7 +2447,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="3" t="s">
         <v>10</v>
       </c>
@@ -2453,7 +2458,7 @@
         <v>12</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E98" s="3" t="n">
         <v>2040</v>
@@ -2465,7 +2470,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="3" t="s">
         <v>10</v>
       </c>
@@ -2476,7 +2481,7 @@
         <v>14</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E99" s="3" t="n">
         <v>2040</v>
@@ -2486,7 +2491,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="3" t="s">
         <v>10</v>
       </c>
@@ -2497,7 +2502,7 @@
         <v>15</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E100" s="3" t="n">
         <v>2040</v>
@@ -2507,7 +2512,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="3" t="s">
         <v>10</v>
       </c>
@@ -2518,7 +2523,7 @@
         <v>16</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E101" s="3" t="n">
         <v>2040</v>
@@ -2528,7 +2533,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="3" t="s">
         <v>10</v>
       </c>
@@ -2539,7 +2544,7 @@
         <v>17</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E102" s="3" t="n">
         <v>2040</v>
@@ -2549,7 +2554,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="3" t="s">
         <v>10</v>
       </c>
@@ -2560,7 +2565,7 @@
         <v>18</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E103" s="3" t="n">
         <v>2040</v>
@@ -2574,13 +2579,13 @@
         <v>10</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E104" s="3" t="n">
         <v>2040</v>
@@ -2595,13 +2600,13 @@
         <v>10</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E105" s="3" t="n">
         <v>2040</v>
@@ -2618,13 +2623,13 @@
         <v>10</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E106" s="3" t="n">
         <v>2040</v>
@@ -2641,13 +2646,13 @@
         <v>10</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E107" s="3" t="n">
         <v>2040</v>
@@ -2661,13 +2666,13 @@
         <v>10</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E108" s="3" t="n">
         <v>2040</v>
@@ -2681,13 +2686,13 @@
         <v>10</v>
       </c>
       <c r="B109" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C109" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C109" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="D109" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E109" s="3" t="n">
         <v>2040</v>
@@ -2704,13 +2709,13 @@
         <v>10</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E110" s="3" t="n">
         <v>2040</v>
@@ -2724,13 +2729,13 @@
         <v>10</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E111" s="3" t="n">
         <v>2040</v>
@@ -2744,13 +2749,13 @@
         <v>10</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E112" s="3" t="n">
         <v>2040</v>
@@ -2765,13 +2770,13 @@
         <v>10</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E113" s="3" t="n">
         <v>2040</v>
@@ -2788,13 +2793,13 @@
         <v>10</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E114" s="3" t="n">
         <v>2040</v>
@@ -2808,13 +2813,13 @@
         <v>10</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E115" s="3" t="n">
         <v>2040</v>
@@ -2828,13 +2833,13 @@
         <v>10</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E116" s="3" t="n">
         <v>2040</v>
@@ -2848,13 +2853,13 @@
         <v>10</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E117" s="3" t="n">
         <v>2040</v>
@@ -2871,13 +2876,13 @@
         <v>10</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E118" s="3" t="n">
         <v>2040</v>
@@ -2894,13 +2899,13 @@
         <v>10</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E119" s="3" t="n">
         <v>2040</v>
@@ -2917,13 +2922,13 @@
         <v>10</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E120" s="3" t="n">
         <v>2040</v>
@@ -2937,13 +2942,13 @@
         <v>10</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E121" s="3" t="n">
         <v>2040</v>
@@ -2957,13 +2962,13 @@
         <v>10</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E122" s="3" t="n">
         <v>2040</v>
@@ -2980,13 +2985,13 @@
         <v>10</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E123" s="3" t="n">
         <v>2040</v>
@@ -3000,13 +3005,13 @@
         <v>10</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E124" s="3" t="n">
         <v>2040</v>
@@ -3020,13 +3025,13 @@
         <v>10</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E125" s="3" t="n">
         <v>2040</v>
@@ -3040,13 +3045,13 @@
         <v>10</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E126" s="3" t="n">
         <v>2040</v>
@@ -3061,13 +3066,13 @@
         <v>10</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E127" s="3" t="n">
         <v>2040</v>
@@ -3081,13 +3086,13 @@
         <v>10</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E128" s="3" t="n">
         <v>2040</v>
@@ -3101,13 +3106,13 @@
         <v>10</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E129" s="3" t="n">
         <v>2040</v>
@@ -3121,13 +3126,13 @@
         <v>10</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E130" s="3" t="n">
         <v>2040</v>
@@ -3144,13 +3149,13 @@
         <v>10</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E131" s="3" t="n">
         <v>2040</v>
@@ -3167,13 +3172,13 @@
         <v>10</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E132" s="3" t="n">
         <v>2040</v>
@@ -3188,13 +3193,13 @@
         <v>10</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E133" s="3" t="n">
         <v>2040</v>
@@ -3208,13 +3213,13 @@
         <v>10</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E134" s="3" t="n">
         <v>2040</v>
@@ -3228,13 +3233,13 @@
         <v>10</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E135" s="3" t="n">
         <v>2040</v>
@@ -3248,13 +3253,13 @@
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D136" s="3" t="s">
         <v>13</v>
@@ -3271,16 +3276,16 @@
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E137" s="3" t="n">
         <v>2040</v>
@@ -3297,7 +3302,7 @@
         <v>10</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>18</v>
@@ -3312,12 +3317,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>18</v>
@@ -3337,13 +3342,13 @@
         <v>10</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E140" s="3" t="n">
         <v>2040</v>
@@ -3354,14 +3359,14 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:J140">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Helsinki_dheat"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="4">
       <filters>
-        <filter val="2025"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Oulu_dheat"/>
+        <filter val="2040"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Added 2030 DH units. Added a correction factor for FI00 DH demand to remove the demand in small DH networks.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-chp.xlsx
+++ b/input/capacity/additional-units-chp.xlsx
@@ -8,11 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Capacity" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Capacity" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$140</definedName>
-  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -23,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="46">
   <si>
     <t xml:space="preserve">Node</t>
   </si>
@@ -280,7 +277,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -288,7 +285,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -296,19 +293,121 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J140"/>
+  <dimension ref="A1:J222"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D150" activeCellId="0" sqref="D150"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A130" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -352,7 +451,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -378,7 +477,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -402,7 +501,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -426,7 +525,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -450,7 +549,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -474,7 +573,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -500,7 +599,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -524,7 +623,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -548,7 +647,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -571,7 +670,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -594,7 +693,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -615,7 +714,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
@@ -638,7 +737,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
@@ -658,7 +757,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
         <v>10</v>
       </c>
@@ -681,7 +780,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
@@ -704,7 +803,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
@@ -724,7 +823,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
@@ -744,7 +843,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
         <v>10</v>
       </c>
@@ -767,7 +866,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
         <v>10</v>
       </c>
@@ -790,7 +889,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
         <v>10</v>
       </c>
@@ -813,7 +912,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
         <v>10</v>
       </c>
@@ -836,7 +935,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
         <v>10</v>
       </c>
@@ -856,7 +955,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
         <v>10</v>
       </c>
@@ -876,7 +975,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
@@ -899,7 +998,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>10</v>
       </c>
@@ -919,7 +1018,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
@@ -942,7 +1041,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
@@ -962,7 +1061,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>10</v>
       </c>
@@ -982,7 +1081,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
@@ -1005,7 +1104,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>10</v>
       </c>
@@ -1028,7 +1127,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>10</v>
       </c>
@@ -1051,7 +1150,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
@@ -1071,7 +1170,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>10</v>
       </c>
@@ -1091,7 +1190,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
@@ -1114,7 +1213,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>32</v>
       </c>
@@ -1137,7 +1236,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>32</v>
       </c>
@@ -1157,7 +1256,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>32</v>
       </c>
@@ -1177,7 +1276,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>34</v>
       </c>
@@ -1197,7 +1296,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>34</v>
       </c>
@@ -1220,7 +1319,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>34</v>
       </c>
@@ -1243,7 +1342,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>34</v>
       </c>
@@ -1266,7 +1365,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>34</v>
       </c>
@@ -1286,7 +1385,7 @@
         <v>4158</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>34</v>
       </c>
@@ -1306,7 +1405,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>36</v>
       </c>
@@ -1329,7 +1428,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>36</v>
       </c>
@@ -1352,7 +1451,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>36</v>
       </c>
@@ -1372,7 +1471,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>36</v>
       </c>
@@ -1392,7 +1491,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>38</v>
       </c>
@@ -1415,7 +1514,7 @@
         <v>7929</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>38</v>
       </c>
@@ -1438,7 +1537,7 @@
         <v>7512</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>38</v>
       </c>
@@ -1461,7 +1560,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>38</v>
       </c>
@@ -1481,7 +1580,7 @@
         <v>23300</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
         <v>40</v>
       </c>
@@ -1504,7 +1603,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>40</v>
       </c>
@@ -1527,7 +1626,7 @@
         <v>10650</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>40</v>
       </c>
@@ -1547,7 +1646,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>40</v>
       </c>
@@ -1567,7 +1666,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>42</v>
       </c>
@@ -1590,7 +1689,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
         <v>42</v>
       </c>
@@ -1613,7 +1712,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>42</v>
       </c>
@@ -1636,7 +1735,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>42</v>
       </c>
@@ -1659,7 +1758,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>42</v>
       </c>
@@ -1679,7 +1778,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>42</v>
       </c>
@@ -1699,7 +1798,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
         <v>42</v>
       </c>
@@ -1719,7 +1818,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>32</v>
       </c>
@@ -1740,7 +1839,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
         <v>32</v>
       </c>
@@ -1763,7 +1862,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
         <v>32</v>
       </c>
@@ -1786,7 +1885,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
         <v>32</v>
       </c>
@@ -1807,7 +1906,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
         <v>32</v>
       </c>
@@ -1828,7 +1927,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
         <v>34</v>
       </c>
@@ -1849,7 +1948,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
         <v>34</v>
       </c>
@@ -1872,7 +1971,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
         <v>34</v>
       </c>
@@ -1895,7 +1994,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
         <v>34</v>
       </c>
@@ -1916,7 +2015,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
         <v>34</v>
       </c>
@@ -1937,7 +2036,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
         <v>36</v>
       </c>
@@ -1957,7 +2056,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
         <v>36</v>
       </c>
@@ -1980,7 +2079,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
         <v>36</v>
       </c>
@@ -2003,7 +2102,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
         <v>36</v>
       </c>
@@ -2023,7 +2122,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
         <v>36</v>
       </c>
@@ -2043,7 +2142,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
         <v>38</v>
       </c>
@@ -2063,7 +2162,7 @@
         <v>16500</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
         <v>38</v>
       </c>
@@ -2086,7 +2185,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
         <v>38</v>
       </c>
@@ -2109,7 +2208,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
         <v>38</v>
       </c>
@@ -2132,7 +2231,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
         <v>38</v>
       </c>
@@ -2152,7 +2251,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
         <v>40</v>
       </c>
@@ -2172,7 +2271,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
         <v>40</v>
       </c>
@@ -2192,7 +2291,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
         <v>40</v>
       </c>
@@ -2215,7 +2314,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
         <v>40</v>
       </c>
@@ -2238,7 +2337,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
         <v>40</v>
       </c>
@@ -2261,7 +2360,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
         <v>40</v>
       </c>
@@ -2281,7 +2380,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
         <v>40</v>
       </c>
@@ -2301,7 +2400,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
         <v>42</v>
       </c>
@@ -2321,7 +2420,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
         <v>42</v>
       </c>
@@ -2341,7 +2440,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
         <v>42</v>
       </c>
@@ -2364,7 +2463,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
         <v>42</v>
       </c>
@@ -2387,7 +2486,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
         <v>42</v>
       </c>
@@ -2407,7 +2506,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
         <v>42</v>
       </c>
@@ -2427,7 +2526,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
         <v>42</v>
       </c>
@@ -2447,7 +2546,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="3" t="s">
         <v>10</v>
       </c>
@@ -2470,7 +2569,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="3" t="s">
         <v>10</v>
       </c>
@@ -2491,7 +2590,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="3" t="s">
         <v>10</v>
       </c>
@@ -2512,7 +2611,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="3" t="s">
         <v>10</v>
       </c>
@@ -2530,10 +2629,10 @@
       </c>
       <c r="F101" s="3"/>
       <c r="G101" s="3" t="n">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="3" t="s">
         <v>10</v>
       </c>
@@ -2554,7 +2653,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="3" t="s">
         <v>10</v>
       </c>
@@ -2574,7 +2673,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="3" t="s">
         <v>10</v>
       </c>
@@ -2595,7 +2694,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="3" t="s">
         <v>10</v>
       </c>
@@ -2618,7 +2717,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="3" t="s">
         <v>10</v>
       </c>
@@ -2641,7 +2740,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="3" t="s">
         <v>10</v>
       </c>
@@ -2661,7 +2760,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="3" t="s">
         <v>10</v>
       </c>
@@ -2681,15 +2780,15 @@
         <v>100</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B109" s="1" t="s">
-        <v>22</v>
+      <c r="B109" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>44</v>
@@ -2698,13 +2797,13 @@
         <v>2040</v>
       </c>
       <c r="F109" s="1" t="n">
-        <v>125</v>
+        <v>20</v>
       </c>
       <c r="G109" s="1" t="n">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="3" t="s">
         <v>10</v>
       </c>
@@ -2712,7 +2811,7 @@
         <v>22</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>44</v>
@@ -2720,11 +2819,14 @@
       <c r="E110" s="3" t="n">
         <v>2040</v>
       </c>
+      <c r="F110" s="1" t="n">
+        <v>125</v>
+      </c>
       <c r="G110" s="1" t="n">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="3" t="s">
         <v>10</v>
       </c>
@@ -2732,7 +2834,7 @@
         <v>22</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>44</v>
@@ -2741,15 +2843,15 @@
         <v>2040</v>
       </c>
       <c r="G111" s="1" t="n">
-        <v>50</v>
+        <v>400</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B112" s="3" t="s">
-        <v>23</v>
+      <c r="B112" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>18</v>
@@ -2760,20 +2862,19 @@
       <c r="E112" s="3" t="n">
         <v>2040</v>
       </c>
-      <c r="F112" s="1"/>
       <c r="G112" s="1" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B113" s="3" t="s">
-        <v>23</v>
+      <c r="B113" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>44</v>
@@ -2781,11 +2882,8 @@
       <c r="E113" s="3" t="n">
         <v>2040</v>
       </c>
-      <c r="F113" s="1" t="n">
-        <v>146</v>
-      </c>
       <c r="G113" s="1" t="n">
-        <v>250</v>
+        <v>30</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2796,7 +2894,7 @@
         <v>23</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>44</v>
@@ -2804,8 +2902,9 @@
       <c r="E114" s="3" t="n">
         <v>2040</v>
       </c>
+      <c r="F114" s="1"/>
       <c r="G114" s="1" t="n">
-        <v>620</v>
+        <v>100</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2816,7 +2915,7 @@
         <v>23</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>44</v>
@@ -2824,8 +2923,11 @@
       <c r="E115" s="3" t="n">
         <v>2040</v>
       </c>
+      <c r="F115" s="1" t="n">
+        <v>146</v>
+      </c>
       <c r="G115" s="1" t="n">
-        <v>150</v>
+        <v>250</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2836,65 +2938,59 @@
         <v>23</v>
       </c>
       <c r="C116" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E116" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G116" s="1" t="n">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E117" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G117" s="1" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C118" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D116" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E116" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="G116" s="1" t="n">
+      <c r="D118" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E118" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G118" s="1" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D117" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E117" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F117" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="G117" s="1" t="n">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D118" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E118" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F118" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="G118" s="1" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="3" t="s">
         <v>10</v>
       </c>
@@ -2902,7 +2998,7 @@
         <v>27</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D119" s="3" t="s">
         <v>44</v>
@@ -2911,13 +3007,13 @@
         <v>2040</v>
       </c>
       <c r="F119" s="1" t="n">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="G119" s="1" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="3" t="s">
         <v>10</v>
       </c>
@@ -2925,7 +3021,7 @@
         <v>27</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D120" s="3" t="s">
         <v>44</v>
@@ -2933,11 +3029,14 @@
       <c r="E120" s="3" t="n">
         <v>2040</v>
       </c>
+      <c r="F120" s="1" t="n">
+        <v>30</v>
+      </c>
       <c r="G120" s="1" t="n">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="3" t="s">
         <v>10</v>
       </c>
@@ -2945,62 +3044,62 @@
         <v>27</v>
       </c>
       <c r="C121" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E121" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F121" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="G121" s="1" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E122" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G122" s="1" t="n">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C123" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D121" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E121" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="G121" s="1" t="n">
+      <c r="D123" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E123" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G123" s="1" t="n">
         <v>200</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D122" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E122" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F122" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="G122" s="1" t="n">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D123" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E123" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="G123" s="1" t="n">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
         <v>10</v>
       </c>
@@ -3008,7 +3107,7 @@
         <v>29</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>44</v>
@@ -3016,11 +3115,14 @@
       <c r="E124" s="3" t="n">
         <v>2040</v>
       </c>
+      <c r="F124" s="1" t="n">
+        <v>100</v>
+      </c>
       <c r="G124" s="1" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="125" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
         <v>10</v>
       </c>
@@ -3028,7 +3130,7 @@
         <v>29</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>44</v>
@@ -3037,7 +3139,7 @@
         <v>2040</v>
       </c>
       <c r="G125" s="1" t="n">
-        <v>50</v>
+        <v>600</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3045,7 +3147,7 @@
         <v>10</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>17</v>
@@ -3056,9 +3158,8 @@
       <c r="E126" s="3" t="n">
         <v>2040</v>
       </c>
-      <c r="F126" s="1"/>
       <c r="G126" s="1" t="n">
-        <v>120</v>
+        <v>80</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3066,10 +3167,10 @@
         <v>10</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>44</v>
@@ -3078,7 +3179,7 @@
         <v>2040</v>
       </c>
       <c r="G127" s="1" t="n">
-        <v>500</v>
+        <v>50</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3089,7 +3190,7 @@
         <v>30</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D128" s="3" t="s">
         <v>44</v>
@@ -3097,8 +3198,9 @@
       <c r="E128" s="3" t="n">
         <v>2040</v>
       </c>
+      <c r="F128" s="1"/>
       <c r="G128" s="1" t="n">
-        <v>240</v>
+        <v>120</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3109,65 +3211,59 @@
         <v>30</v>
       </c>
       <c r="C129" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E129" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G129" s="1" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E130" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G130" s="1" t="n">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C131" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D129" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E129" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="G129" s="1" t="n">
+      <c r="D131" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E131" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G131" s="1" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D130" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E130" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F130" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="G130" s="1" t="n">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D131" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E131" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F131" s="1" t="n">
-        <v>400</v>
-      </c>
-      <c r="G131" s="1" t="n">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
         <v>10</v>
       </c>
@@ -3175,7 +3271,7 @@
         <v>31</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D132" s="3" t="s">
         <v>44</v>
@@ -3183,12 +3279,14 @@
       <c r="E132" s="3" t="n">
         <v>2040</v>
       </c>
-      <c r="F132" s="1"/>
+      <c r="F132" s="1" t="n">
+        <v>35</v>
+      </c>
       <c r="G132" s="1" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
         <v>10</v>
       </c>
@@ -3196,7 +3294,7 @@
         <v>31</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D133" s="3" t="s">
         <v>44</v>
@@ -3204,11 +3302,14 @@
       <c r="E133" s="3" t="n">
         <v>2040</v>
       </c>
+      <c r="F133" s="1" t="n">
+        <v>400</v>
+      </c>
       <c r="G133" s="1" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
         <v>10</v>
       </c>
@@ -3216,70 +3317,65 @@
         <v>31</v>
       </c>
       <c r="C134" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E134" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F134" s="1"/>
+      <c r="G134" s="1" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D135" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E135" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G135" s="1" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C136" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D134" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E134" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="G134" s="1" t="n">
+      <c r="D136" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E136" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G136" s="1" t="n">
         <v>1000</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B135" s="1" t="s">
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B137" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C135" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D135" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E135" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F135" s="1" t="n">
-        <v>1400</v>
-      </c>
-      <c r="G135" s="1" t="n">
-        <v>2800</v>
-      </c>
-    </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D136" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E136" s="3" t="n">
-        <v>2025</v>
-      </c>
-      <c r="F136" s="1" t="n">
-        <v>586</v>
-      </c>
-      <c r="G136" s="1" t="n">
-        <v>1172</v>
-      </c>
-    </row>
-    <row r="137" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>26</v>
@@ -3291,53 +3387,59 @@
         <v>2040</v>
       </c>
       <c r="F137" s="1" t="n">
+        <v>1400</v>
+      </c>
+      <c r="G137" s="1" t="n">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E138" s="3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F138" s="1" t="n">
         <v>586</v>
       </c>
-      <c r="G137" s="1" t="n">
+      <c r="G138" s="1" t="n">
         <v>1172</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D138" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E138" s="3" t="n">
-        <v>2025</v>
-      </c>
-      <c r="G138" s="1" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="1" t="s">
-        <v>10</v>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="E139" s="3" t="n">
-        <v>2025</v>
+        <v>2040</v>
+      </c>
+      <c r="F139" s="1" t="n">
+        <v>586</v>
       </c>
       <c r="G139" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
         <v>10</v>
       </c>
@@ -3348,29 +3450,1707 @@
         <v>18</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="E140" s="3" t="n">
-        <v>2040</v>
+        <v>2025</v>
       </c>
       <c r="G140" s="1" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E141" s="3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G141" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E142" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G142" s="1" t="n">
         <v>250</v>
       </c>
     </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E143" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F143" s="3" t="n">
+        <v>470</v>
+      </c>
+      <c r="G143" s="3" t="n">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E144" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F144" s="3"/>
+      <c r="G144" s="3" t="n">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E145" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F145" s="3"/>
+      <c r="G145" s="3" t="n">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D146" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E146" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F146" s="3"/>
+      <c r="G146" s="3" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E147" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F147" s="3"/>
+      <c r="G147" s="3" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D148" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E148" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F148" s="3"/>
+      <c r="G148" s="3" t="n">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E149" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F149" s="3"/>
+      <c r="G149" s="3" t="n">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E150" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F150" s="3"/>
+      <c r="G150" s="3" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E151" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F151" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="G151" s="1" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E152" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F152" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="G152" s="1" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D153" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E153" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G153" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E154" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G154" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D155" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E155" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F155" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="G155" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D156" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E156" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F156" s="1" t="n">
+        <v>280</v>
+      </c>
+      <c r="G156" s="1" t="n">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D157" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E157" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G157" s="1" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E158" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G158" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D159" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E159" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F159" s="1"/>
+      <c r="G159" s="1" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D160" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E160" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F160" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="G160" s="1" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D161" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E161" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G161" s="1" t="n">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D162" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E162" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G162" s="1" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D163" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E163" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G163" s="1" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D164" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E164" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F164" s="1" t="n">
+        <v>1400</v>
+      </c>
+      <c r="G164" s="1" t="n">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E165" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F165" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="G165" s="1" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D166" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E166" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F166" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G166" s="1" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D167" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E167" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F167" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="G167" s="1" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D168" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E168" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G168" s="1" t="n">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D169" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E169" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G169" s="1" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E170" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G170" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D171" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E171" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F171" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="G171" s="1" t="n">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D172" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E172" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G172" s="1" t="n">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D173" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E173" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G173" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D174" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E174" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G174" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E175" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F175" s="1"/>
+      <c r="G175" s="1" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E176" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G176" s="1" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D177" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E177" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G177" s="1" t="n">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D178" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E178" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F178" s="1" t="n">
+        <v>234</v>
+      </c>
+      <c r="G178" s="1" t="n">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E179" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F179" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="G179" s="1" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D180" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E180" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F180" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="G180" s="1" t="n">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D181" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E181" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F181" s="1"/>
+      <c r="G181" s="1" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D182" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E182" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G182" s="1" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D183" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E183" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G183" s="1" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D184" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E184" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F184" s="1"/>
+      <c r="G184" s="1" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E185" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F185" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="G185" s="1" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E186" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F186" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="G186" s="1" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D187" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E187" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F187" s="1"/>
+      <c r="G187" s="1" t="n">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D188" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E188" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F188" s="1"/>
+      <c r="G188" s="1" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D189" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E189" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F189" s="1"/>
+      <c r="G189" s="1" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D190" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E190" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F190" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="G190" s="1" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D191" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E191" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F191" s="1" t="n">
+        <v>450</v>
+      </c>
+      <c r="G191" s="1" t="n">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D192" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E192" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F192" s="1"/>
+      <c r="G192" s="1" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D193" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E193" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F193" s="1"/>
+      <c r="G193" s="1" t="n">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D194" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E194" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G194" s="1" t="n">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D195" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E195" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F195" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="G195" s="1" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D196" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E196" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F196" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="G196" s="1" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D197" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E197" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G197" s="1" t="n">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D198" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E198" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G198" s="1" t="n">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D199" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E199" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G199" s="1" t="n">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D200" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E200" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F200" s="1" t="n">
+        <v>3000</v>
+      </c>
+      <c r="G200" s="1" t="n">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D201" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E201" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F201" s="1" t="n">
+        <v>3000</v>
+      </c>
+      <c r="G201" s="1" t="n">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D202" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E202" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F202" s="1" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G202" s="1" t="n">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D203" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E203" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G203" s="1" t="n">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D204" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E204" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F204" s="1" t="n">
+        <v>6000</v>
+      </c>
+      <c r="G204" s="1" t="n">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D205" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E205" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G205" s="1" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D206" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E206" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G206" s="1" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D207" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E207" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F207" s="1" t="n">
+        <v>850</v>
+      </c>
+      <c r="G207" s="1" t="n">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D208" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E208" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F208" s="1" t="n">
+        <v>850</v>
+      </c>
+      <c r="G208" s="1" t="n">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D209" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E209" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F209" s="1" t="n">
+        <v>3500</v>
+      </c>
+      <c r="G209" s="1" t="n">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D210" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E210" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G210" s="1" t="n">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D211" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E211" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G211" s="1" t="n">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D212" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E212" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G212" s="1" t="n">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D213" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E213" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G213" s="1" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D214" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E214" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F214" s="1" t="n">
+        <v>320</v>
+      </c>
+      <c r="G214" s="1" t="n">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D215" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E215" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F215" s="1" t="n">
+        <v>900</v>
+      </c>
+      <c r="G215" s="1" t="n">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D216" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E216" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G216" s="1" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D217" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E217" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G217" s="1" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D218" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E218" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G218" s="1" t="n">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D219" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E219" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F219" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="G219" s="1" t="n">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C222" s="0"/>
+      <c r="D222" s="0"/>
+      <c r="G222" s="0"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J140">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="2040"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Espoo_dheat"/>
-        <filter val="Turku_dheat"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3378,6 +5158,5 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added modifications to Distributed Energy 2030 scenario. Capacity, demand, fuelprices, EV fleet.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-chp.xlsx
+++ b/input/capacity/additional-units-chp.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Capacity" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$219</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="46">
   <si>
     <t xml:space="preserve">Node</t>
   </si>
@@ -293,6 +296,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
@@ -401,13 +408,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J222"/>
+  <dimension ref="A1:J220"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A130" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G227" activeCellId="0" sqref="G227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -451,7 +458,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -477,7 +484,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -501,7 +508,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -525,7 +532,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -549,7 +556,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -573,7 +580,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -599,7 +606,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -623,7 +630,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -647,7 +654,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -670,7 +677,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -693,7 +700,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -714,7 +721,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
@@ -737,7 +744,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
@@ -757,7 +764,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
         <v>10</v>
       </c>
@@ -780,7 +787,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
@@ -803,7 +810,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
@@ -823,7 +830,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
@@ -866,7 +873,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
         <v>10</v>
       </c>
@@ -889,7 +896,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
         <v>10</v>
       </c>
@@ -912,7 +919,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
         <v>10</v>
       </c>
@@ -935,7 +942,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
         <v>10</v>
       </c>
@@ -955,7 +962,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
         <v>10</v>
       </c>
@@ -975,7 +982,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
@@ -998,7 +1005,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>10</v>
       </c>
@@ -1018,7 +1025,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
@@ -1041,7 +1048,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
@@ -1061,7 +1068,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>10</v>
       </c>
@@ -1081,7 +1088,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
@@ -1104,7 +1111,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>10</v>
       </c>
@@ -1127,7 +1134,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>10</v>
       </c>
@@ -1150,7 +1157,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
@@ -1170,7 +1177,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>10</v>
       </c>
@@ -1190,7 +1197,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
@@ -1213,7 +1220,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>32</v>
       </c>
@@ -1236,7 +1243,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>32</v>
       </c>
@@ -1256,7 +1263,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>32</v>
       </c>
@@ -1276,7 +1283,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>34</v>
       </c>
@@ -1296,7 +1303,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>34</v>
       </c>
@@ -1319,7 +1326,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>34</v>
       </c>
@@ -1342,7 +1349,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>34</v>
       </c>
@@ -1365,7 +1372,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>34</v>
       </c>
@@ -1385,7 +1392,7 @@
         <v>4158</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>34</v>
       </c>
@@ -1405,7 +1412,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>36</v>
       </c>
@@ -1428,7 +1435,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>36</v>
       </c>
@@ -1451,7 +1458,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>36</v>
       </c>
@@ -1471,7 +1478,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>36</v>
       </c>
@@ -1491,7 +1498,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>38</v>
       </c>
@@ -1514,7 +1521,7 @@
         <v>7929</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>38</v>
       </c>
@@ -1537,7 +1544,7 @@
         <v>7512</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>38</v>
       </c>
@@ -1560,7 +1567,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>38</v>
       </c>
@@ -1580,7 +1587,7 @@
         <v>23300</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
         <v>40</v>
       </c>
@@ -1603,7 +1610,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>40</v>
       </c>
@@ -1626,7 +1633,7 @@
         <v>10650</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>40</v>
       </c>
@@ -1646,7 +1653,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>40</v>
       </c>
@@ -1666,7 +1673,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>42</v>
       </c>
@@ -1689,7 +1696,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
         <v>42</v>
       </c>
@@ -1712,7 +1719,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>42</v>
       </c>
@@ -1735,7 +1742,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>42</v>
       </c>
@@ -1758,7 +1765,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>42</v>
       </c>
@@ -1778,7 +1785,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>42</v>
       </c>
@@ -1798,7 +1805,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
         <v>42</v>
       </c>
@@ -1818,7 +1825,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>32</v>
       </c>
@@ -1839,7 +1846,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
         <v>32</v>
       </c>
@@ -1862,7 +1869,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
         <v>32</v>
       </c>
@@ -1885,7 +1892,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
         <v>32</v>
       </c>
@@ -1906,7 +1913,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
         <v>32</v>
       </c>
@@ -1927,7 +1934,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
         <v>34</v>
       </c>
@@ -1948,7 +1955,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
         <v>34</v>
       </c>
@@ -1971,7 +1978,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
         <v>34</v>
       </c>
@@ -1994,7 +2001,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
         <v>34</v>
       </c>
@@ -2015,7 +2022,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
         <v>34</v>
       </c>
@@ -2036,7 +2043,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
         <v>36</v>
       </c>
@@ -2056,7 +2063,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
         <v>36</v>
       </c>
@@ -2079,7 +2086,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
         <v>36</v>
       </c>
@@ -2102,7 +2109,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
         <v>36</v>
       </c>
@@ -2122,7 +2129,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
         <v>36</v>
       </c>
@@ -2142,7 +2149,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
         <v>38</v>
       </c>
@@ -2162,7 +2169,7 @@
         <v>16500</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
         <v>38</v>
       </c>
@@ -2185,7 +2192,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
         <v>38</v>
       </c>
@@ -2208,7 +2215,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
         <v>38</v>
       </c>
@@ -2231,7 +2238,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
         <v>38</v>
       </c>
@@ -2251,7 +2258,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
         <v>40</v>
       </c>
@@ -2271,7 +2278,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
         <v>40</v>
       </c>
@@ -2291,7 +2298,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
         <v>40</v>
       </c>
@@ -2314,7 +2321,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
         <v>40</v>
       </c>
@@ -2337,7 +2344,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
         <v>40</v>
       </c>
@@ -2360,7 +2367,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
         <v>40</v>
       </c>
@@ -2380,7 +2387,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
         <v>40</v>
       </c>
@@ -2400,7 +2407,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
         <v>42</v>
       </c>
@@ -2420,7 +2427,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
         <v>42</v>
       </c>
@@ -2440,7 +2447,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
         <v>42</v>
       </c>
@@ -2463,7 +2470,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
         <v>42</v>
       </c>
@@ -2486,7 +2493,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
         <v>42</v>
       </c>
@@ -2506,7 +2513,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
         <v>42</v>
       </c>
@@ -2526,7 +2533,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
         <v>42</v>
       </c>
@@ -2546,7 +2553,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="3" t="s">
         <v>10</v>
       </c>
@@ -2569,7 +2576,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="3" t="s">
         <v>10</v>
       </c>
@@ -2590,7 +2597,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="3" t="s">
         <v>10</v>
       </c>
@@ -2611,7 +2618,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="3" t="s">
         <v>10</v>
       </c>
@@ -2632,7 +2639,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="3" t="s">
         <v>10</v>
       </c>
@@ -2653,7 +2660,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="3" t="s">
         <v>10</v>
       </c>
@@ -2673,7 +2680,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="3" t="s">
         <v>10</v>
       </c>
@@ -2694,7 +2701,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="3" t="s">
         <v>10</v>
       </c>
@@ -2717,7 +2724,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="3" t="s">
         <v>10</v>
       </c>
@@ -2740,7 +2747,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="3" t="s">
         <v>10</v>
       </c>
@@ -2760,7 +2767,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="3" t="s">
         <v>10</v>
       </c>
@@ -2780,7 +2787,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="s">
         <v>10</v>
       </c>
@@ -2803,7 +2810,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="3" t="s">
         <v>10</v>
       </c>
@@ -2826,7 +2833,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="3" t="s">
         <v>10</v>
       </c>
@@ -2846,7 +2853,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="3" t="s">
         <v>10</v>
       </c>
@@ -2866,7 +2873,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="3" t="s">
         <v>10</v>
       </c>
@@ -2886,7 +2893,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="3" t="s">
         <v>10</v>
       </c>
@@ -2907,7 +2914,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="3" t="s">
         <v>10</v>
       </c>
@@ -2930,7 +2937,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="3" t="s">
         <v>10</v>
       </c>
@@ -2950,7 +2957,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="3" t="s">
         <v>10</v>
       </c>
@@ -2970,7 +2977,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="3" t="s">
         <v>10</v>
       </c>
@@ -2990,7 +2997,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="3" t="s">
         <v>10</v>
       </c>
@@ -3013,7 +3020,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="3" t="s">
         <v>10</v>
       </c>
@@ -3036,7 +3043,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="3" t="s">
         <v>10</v>
       </c>
@@ -3059,7 +3066,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="3" t="s">
         <v>10</v>
       </c>
@@ -3079,7 +3086,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="3" t="s">
         <v>10</v>
       </c>
@@ -3099,7 +3106,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
         <v>10</v>
       </c>
@@ -3122,7 +3129,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
         <v>10</v>
       </c>
@@ -3142,7 +3149,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
         <v>10</v>
       </c>
@@ -3162,7 +3169,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
         <v>10</v>
       </c>
@@ -3182,7 +3189,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
         <v>10</v>
       </c>
@@ -3203,7 +3210,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
         <v>10</v>
       </c>
@@ -3223,7 +3230,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
         <v>10</v>
       </c>
@@ -3243,7 +3250,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
         <v>10</v>
       </c>
@@ -3263,7 +3270,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
         <v>10</v>
       </c>
@@ -3286,7 +3293,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
         <v>10</v>
       </c>
@@ -3309,7 +3316,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
         <v>10</v>
       </c>
@@ -3330,7 +3337,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
         <v>10</v>
       </c>
@@ -3350,7 +3357,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
         <v>10</v>
       </c>
@@ -3439,7 +3446,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
         <v>10</v>
       </c>
@@ -3459,7 +3466,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
         <v>10</v>
       </c>
@@ -3479,7 +3486,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
         <v>10</v>
       </c>
@@ -3499,7 +3506,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="3" t="s">
         <v>10</v>
       </c>
@@ -3522,7 +3529,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="3" t="s">
         <v>10</v>
       </c>
@@ -3543,7 +3550,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="3" t="s">
         <v>10</v>
       </c>
@@ -3564,7 +3571,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="3" t="s">
         <v>10</v>
       </c>
@@ -3585,7 +3592,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="3" t="s">
         <v>10</v>
       </c>
@@ -3606,7 +3613,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="3" t="s">
         <v>10</v>
       </c>
@@ -3627,7 +3634,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="3" t="s">
         <v>10</v>
       </c>
@@ -3648,7 +3655,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="3" t="s">
         <v>10</v>
       </c>
@@ -3669,7 +3676,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="3" t="s">
         <v>10</v>
       </c>
@@ -3692,7 +3699,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="3" t="s">
         <v>10</v>
       </c>
@@ -3715,7 +3722,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="3" t="s">
         <v>10</v>
       </c>
@@ -3735,7 +3742,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="3" t="s">
         <v>10</v>
       </c>
@@ -3755,7 +3762,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="3" t="s">
         <v>10</v>
       </c>
@@ -3778,7 +3785,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="3" t="s">
         <v>10</v>
       </c>
@@ -3801,7 +3808,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="3" t="s">
         <v>10</v>
       </c>
@@ -3821,7 +3828,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="3" t="s">
         <v>10</v>
       </c>
@@ -3841,7 +3848,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="3" t="s">
         <v>10</v>
       </c>
@@ -3862,7 +3869,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="3" t="s">
         <v>10</v>
       </c>
@@ -3885,7 +3892,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="3" t="s">
         <v>10</v>
       </c>
@@ -3905,7 +3912,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="3" t="s">
         <v>10</v>
       </c>
@@ -3925,7 +3932,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="3" t="s">
         <v>10</v>
       </c>
@@ -3968,7 +3975,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="3" t="s">
         <v>10</v>
       </c>
@@ -3991,7 +3998,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="3" t="s">
         <v>10</v>
       </c>
@@ -4014,7 +4021,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="3" t="s">
         <v>10</v>
       </c>
@@ -4037,7 +4044,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="3" t="s">
         <v>10</v>
       </c>
@@ -4057,7 +4064,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="3" t="s">
         <v>10</v>
       </c>
@@ -4077,7 +4084,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="3" t="s">
         <v>10</v>
       </c>
@@ -4097,7 +4104,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="s">
         <v>10</v>
       </c>
@@ -4120,7 +4127,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="s">
         <v>10</v>
       </c>
@@ -4140,7 +4147,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="s">
         <v>10</v>
       </c>
@@ -4160,7 +4167,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="1" t="s">
         <v>10</v>
       </c>
@@ -4180,7 +4187,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1" t="s">
         <v>10</v>
       </c>
@@ -4201,7 +4208,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="s">
         <v>10</v>
       </c>
@@ -4221,7 +4228,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="s">
         <v>10</v>
       </c>
@@ -4241,7 +4248,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="s">
         <v>10</v>
       </c>
@@ -4264,7 +4271,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="s">
         <v>10</v>
       </c>
@@ -4287,7 +4294,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="s">
         <v>10</v>
       </c>
@@ -4310,7 +4317,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="s">
         <v>10</v>
       </c>
@@ -4331,7 +4338,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="s">
         <v>10</v>
       </c>
@@ -4351,7 +4358,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="s">
         <v>10</v>
       </c>
@@ -4371,7 +4378,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="1" t="s">
         <v>32</v>
       </c>
@@ -4392,7 +4399,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="s">
         <v>32</v>
       </c>
@@ -4415,7 +4422,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="s">
         <v>32</v>
       </c>
@@ -4438,7 +4445,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="s">
         <v>32</v>
       </c>
@@ -4459,7 +4466,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="s">
         <v>32</v>
       </c>
@@ -4480,7 +4487,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="s">
         <v>34</v>
       </c>
@@ -4501,7 +4508,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="s">
         <v>34</v>
       </c>
@@ -4524,7 +4531,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="s">
         <v>34</v>
       </c>
@@ -4547,7 +4554,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="s">
         <v>34</v>
       </c>
@@ -4568,7 +4575,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="1" t="s">
         <v>34</v>
       </c>
@@ -4589,7 +4596,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="s">
         <v>36</v>
       </c>
@@ -4609,7 +4616,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="s">
         <v>36</v>
       </c>
@@ -4632,7 +4639,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="s">
         <v>36</v>
       </c>
@@ -4655,7 +4662,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="s">
         <v>36</v>
       </c>
@@ -4675,7 +4682,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="s">
         <v>36</v>
       </c>
@@ -4695,7 +4702,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="s">
         <v>38</v>
       </c>
@@ -4715,7 +4722,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="1" t="s">
         <v>38</v>
       </c>
@@ -4738,7 +4745,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="s">
         <v>38</v>
       </c>
@@ -4761,7 +4768,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="1" t="s">
         <v>38</v>
       </c>
@@ -4784,7 +4791,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="1" t="s">
         <v>38</v>
       </c>
@@ -4804,7 +4811,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="1" t="s">
         <v>38</v>
       </c>
@@ -4827,7 +4834,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
         <v>40</v>
       </c>
@@ -4847,7 +4854,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="s">
         <v>40</v>
       </c>
@@ -4867,7 +4874,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="207" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="s">
         <v>40</v>
       </c>
@@ -4890,7 +4897,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="1" t="s">
         <v>40</v>
       </c>
@@ -4913,7 +4920,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="209" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="1" t="s">
         <v>40</v>
       </c>
@@ -4936,7 +4943,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="s">
         <v>40</v>
       </c>
@@ -4956,7 +4963,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="s">
         <v>40</v>
       </c>
@@ -4976,7 +4983,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="212" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="s">
         <v>42</v>
       </c>
@@ -4996,7 +5003,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="213" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="s">
         <v>42</v>
       </c>
@@ -5016,7 +5023,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="214" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="1" t="s">
         <v>42</v>
       </c>
@@ -5039,7 +5046,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="215" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="1" t="s">
         <v>42</v>
       </c>
@@ -5062,7 +5069,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="216" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="s">
         <v>42</v>
       </c>
@@ -5082,7 +5089,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="217" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="1" t="s">
         <v>42</v>
       </c>
@@ -5102,7 +5109,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="218" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="1" t="s">
         <v>42</v>
       </c>
@@ -5122,7 +5129,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="1" t="s">
         <v>42</v>
       </c>
@@ -5138,19 +5145,44 @@
       <c r="E219" s="3" t="n">
         <v>2030</v>
       </c>
-      <c r="F219" s="0" t="n">
+      <c r="F219" s="1" t="n">
         <v>300</v>
       </c>
       <c r="G219" s="1" t="n">
         <v>600</v>
       </c>
     </row>
-    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C222" s="0"/>
-      <c r="D222" s="0"/>
-      <c r="G222" s="0"/>
+    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D220" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E220" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F220" s="0" t="n">
+        <v>586</v>
+      </c>
+      <c r="G220" s="1" t="n">
+        <v>1172</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J219">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Kraft process recovery boiler"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -5158,5 +5190,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated DKW1 electrolysis and UK00 offshore wind.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-chp.xlsx
+++ b/input/capacity/additional-units-chp.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Capacity" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$219</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$220</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">Coal CHP</t>
   </si>
   <si>
-    <t xml:space="preserve">FI00industry</t>
+    <t xml:space="preserve">FI00_industry</t>
   </si>
   <si>
     <t xml:space="preserve">Kraft process recovery boiler</t>
@@ -414,7 +414,7 @@
   <dimension ref="A1:J220"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G227" activeCellId="0" sqref="G227"/>
+      <selection pane="topLeft" activeCell="B223" activeCellId="0" sqref="B223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -867,10 +867,10 @@
         <v>2025</v>
       </c>
       <c r="F19" s="1" t="n">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="G19" s="1" t="n">
-        <v>2800</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3394,13 +3394,13 @@
         <v>2040</v>
       </c>
       <c r="F137" s="1" t="n">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="G137" s="1" t="n">
-        <v>2800</v>
-      </c>
-    </row>
-    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="3" t="s">
         <v>34</v>
       </c>
@@ -3423,7 +3423,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="3" t="s">
         <v>34</v>
       </c>
@@ -3969,10 +3969,10 @@
         <v>2030</v>
       </c>
       <c r="F164" s="1" t="n">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="G164" s="1" t="n">
-        <v>2800</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5152,7 +5152,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="220" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="3" t="s">
         <v>34</v>
       </c>
@@ -5168,7 +5168,7 @@
       <c r="E220" s="3" t="n">
         <v>2030</v>
       </c>
-      <c r="F220" s="0" t="n">
+      <c r="F220" s="1" t="n">
         <v>586</v>
       </c>
       <c r="G220" s="1" t="n">
@@ -5176,10 +5176,15 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J219">
+  <autoFilter ref="A1:J220">
     <filterColumn colId="2">
       <filters>
         <filter val="Kraft process recovery boiler"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="1">
+      <filters>
+        <filter val="FI00industry"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Update capacities and electricity demand 2030.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-chp.xlsx
+++ b/input/capacity/additional-units-chp.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="46">
   <si>
     <t xml:space="preserve">Node</t>
   </si>
@@ -411,10 +411,10 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J220"/>
+  <dimension ref="A1:J221"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B223" activeCellId="0" sqref="B223"/>
+      <selection pane="topLeft" activeCell="D226" activeCellId="0" sqref="D226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -850,7 +850,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
         <v>10</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>10</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>10</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>10</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
         <v>10</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
         <v>10</v>
       </c>
@@ -3316,7 +3316,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
         <v>10</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
         <v>10</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
         <v>10</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="3" t="s">
         <v>10</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
         <v>10</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
         <v>10</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>2040</v>
       </c>
       <c r="G142" s="1" t="n">
-        <v>250</v>
+        <v>350</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3952,7 +3952,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="3" t="s">
         <v>10</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="s">
         <v>10</v>
       </c>
@@ -4294,7 +4294,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="s">
         <v>10</v>
       </c>
@@ -4317,7 +4317,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="s">
         <v>10</v>
       </c>
@@ -4338,7 +4338,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="s">
         <v>10</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="s">
         <v>10</v>
       </c>
@@ -5175,16 +5175,31 @@
         <v>1172</v>
       </c>
     </row>
+    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D221" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E221" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G221" s="1" t="n">
+        <v>250</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J220">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Kraft process recovery boiler"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="1">
       <filters>
-        <filter val="FI00industry"/>
+        <filter val="FI00_others_dheat"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Added some electric boilers FI.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-chp.xlsx
+++ b/input/capacity/additional-units-chp.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Capacity" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$220</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$221</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -414,7 +414,7 @@
   <dimension ref="A1:J221"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D226" activeCellId="0" sqref="D226"/>
+      <selection pane="topLeft" activeCell="C114" activeCellId="0" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -764,7 +764,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
         <v>10</v>
       </c>
@@ -787,7 +787,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
@@ -810,7 +810,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
@@ -830,7 +830,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>10</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>10</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>10</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>2040</v>
       </c>
       <c r="G103" s="1" t="n">
-        <v>250</v>
+        <v>350</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2870,7 +2870,7 @@
         <v>2040</v>
       </c>
       <c r="G112" s="1" t="n">
-        <v>50</v>
+        <v>90</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2893,7 +2893,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="3" t="s">
         <v>10</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="3" t="s">
         <v>10</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="3" t="s">
         <v>10</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="3" t="s">
         <v>10</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="3" t="s">
         <v>10</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>2040</v>
       </c>
       <c r="G127" s="1" t="n">
-        <v>50</v>
+        <v>90</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3267,10 +3267,10 @@
         <v>2040</v>
       </c>
       <c r="G131" s="1" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
         <v>10</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
         <v>10</v>
       </c>
@@ -3316,7 +3316,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
         <v>10</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
         <v>10</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
         <v>10</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
         <v>10</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
         <v>10</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>2040</v>
       </c>
       <c r="G142" s="1" t="n">
-        <v>350</v>
+        <v>600</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3848,7 +3848,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="3" t="s">
         <v>10</v>
       </c>
@@ -3869,7 +3869,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="3" t="s">
         <v>10</v>
       </c>
@@ -3892,7 +3892,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="3" t="s">
         <v>10</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="3" t="s">
         <v>10</v>
       </c>
@@ -3932,7 +3932,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="3" t="s">
         <v>10</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="s">
         <v>10</v>
       </c>
@@ -4294,7 +4294,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="s">
         <v>10</v>
       </c>
@@ -4317,7 +4317,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="s">
         <v>10</v>
       </c>
@@ -4338,7 +4338,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="s">
         <v>10</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="s">
         <v>10</v>
       </c>
@@ -5175,7 +5175,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="221" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="1" t="s">
         <v>10</v>
       </c>
@@ -5196,10 +5196,10 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J220">
+  <autoFilter ref="A1:J221">
     <filterColumn colId="1">
       <filters>
-        <filter val="FI00_others_dheat"/>
+        <filter val="Turku_dheat"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Increased elysis in FR00 2040.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-chp.xlsx
+++ b/input/capacity/additional-units-chp.xlsx
@@ -414,7 +414,7 @@
   <dimension ref="A1:J221"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C114" activeCellId="0" sqref="C114"/>
+      <selection pane="topLeft" activeCell="K104" activeCellId="0" sqref="K104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -606,7 +606,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -630,7 +630,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -654,7 +654,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -677,7 +677,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -700,7 +700,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -764,7 +764,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
         <v>10</v>
       </c>
@@ -787,7 +787,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
@@ -810,7 +810,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
@@ -830,7 +830,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="3" t="s">
         <v>10</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="3" t="s">
         <v>10</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="3" t="s">
         <v>10</v>
       </c>
@@ -2747,7 +2747,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="3" t="s">
         <v>10</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="3" t="s">
         <v>10</v>
       </c>
@@ -2784,10 +2784,10 @@
         <v>2040</v>
       </c>
       <c r="G108" s="1" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="s">
         <v>10</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="3" t="s">
         <v>10</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="3" t="s">
         <v>10</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="3" t="s">
         <v>10</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="3" t="s">
         <v>10</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="3" t="s">
         <v>10</v>
       </c>
@@ -3634,7 +3634,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="3" t="s">
         <v>10</v>
       </c>
@@ -3655,7 +3655,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="3" t="s">
         <v>10</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="3" t="s">
         <v>10</v>
       </c>
@@ -3699,7 +3699,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="3" t="s">
         <v>10</v>
       </c>
@@ -3722,7 +3722,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="3" t="s">
         <v>10</v>
       </c>
@@ -3742,7 +3742,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="3" t="s">
         <v>10</v>
       </c>
@@ -3762,7 +3762,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="3" t="s">
         <v>10</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="3" t="s">
         <v>10</v>
       </c>
@@ -3869,7 +3869,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="3" t="s">
         <v>10</v>
       </c>
@@ -3892,7 +3892,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="3" t="s">
         <v>10</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="3" t="s">
         <v>10</v>
       </c>
@@ -3932,7 +3932,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="3" t="s">
         <v>10</v>
       </c>
@@ -5199,7 +5199,7 @@
   <autoFilter ref="A1:J221">
     <filterColumn colId="1">
       <filters>
-        <filter val="Turku_dheat"/>
+        <filter val="Tampere_dheat"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Added technology for heat storages.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-chp.xlsx
+++ b/input/capacity/additional-units-chp.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="48">
   <si>
     <t xml:space="preserve">Node</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t xml:space="preserve">SE03_industry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heat storage discharger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heat storage charger</t>
   </si>
 </sst>
 </file>
@@ -411,10 +417,10 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J221"/>
+  <dimension ref="A1:J223"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K104" activeCellId="0" sqref="K104"/>
+      <selection pane="topLeft" activeCell="H224" activeCellId="0" sqref="H224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -458,7 +464,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -484,7 +490,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -508,7 +514,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -532,7 +538,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -556,7 +562,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -580,7 +586,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -606,7 +612,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -630,7 +636,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -654,7 +660,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -677,7 +683,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -700,7 +706,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -2553,7 +2559,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="3" t="s">
         <v>10</v>
       </c>
@@ -2576,7 +2582,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="3" t="s">
         <v>10</v>
       </c>
@@ -2597,7 +2603,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="3" t="s">
         <v>10</v>
       </c>
@@ -2618,7 +2624,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="3" t="s">
         <v>10</v>
       </c>
@@ -2639,7 +2645,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="3" t="s">
         <v>10</v>
       </c>
@@ -2660,7 +2666,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="3" t="s">
         <v>10</v>
       </c>
@@ -2680,7 +2686,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="3" t="s">
         <v>10</v>
       </c>
@@ -2701,7 +2707,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="3" t="s">
         <v>10</v>
       </c>
@@ -2724,7 +2730,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="3" t="s">
         <v>10</v>
       </c>
@@ -2747,7 +2753,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="3" t="s">
         <v>10</v>
       </c>
@@ -2767,7 +2773,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="3" t="s">
         <v>10</v>
       </c>
@@ -2787,7 +2793,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="s">
         <v>10</v>
       </c>
@@ -3506,7 +3512,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="3" t="s">
         <v>10</v>
       </c>
@@ -3529,7 +3535,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="3" t="s">
         <v>10</v>
       </c>
@@ -3550,7 +3556,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="3" t="s">
         <v>10</v>
       </c>
@@ -3571,7 +3577,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="3" t="s">
         <v>10</v>
       </c>
@@ -3592,7 +3598,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="3" t="s">
         <v>10</v>
       </c>
@@ -3613,7 +3619,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="3" t="s">
         <v>10</v>
       </c>
@@ -3634,7 +3640,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="3" t="s">
         <v>10</v>
       </c>
@@ -3655,7 +3661,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="3" t="s">
         <v>10</v>
       </c>
@@ -3676,7 +3682,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="3" t="s">
         <v>10</v>
       </c>
@@ -3699,7 +3705,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="3" t="s">
         <v>10</v>
       </c>
@@ -3722,7 +3728,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="3" t="s">
         <v>10</v>
       </c>
@@ -3742,7 +3748,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="3" t="s">
         <v>10</v>
       </c>
@@ -3762,7 +3768,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="3" t="s">
         <v>10</v>
       </c>
@@ -5193,13 +5199,53 @@
       </c>
       <c r="G221" s="1" t="n">
         <v>250</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B222" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D222" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E222" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G222" s="1" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B223" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D223" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E223" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H223" s="1" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J221">
     <filterColumn colId="1">
       <filters>
-        <filter val="Tampere_dheat"/>
+        <filter val="Helsinki_dheat"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>